<commit_message>
Plus Asset and Something zakup
</commit_message>
<xml_diff>
--- a/RhythmGame/Assets/Scripts/Ozi's Scene/메뉴얼.xlsx
+++ b/RhythmGame/Assets/Scripts/Ozi's Scene/메뉴얼.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Github Project\GameJamRhythmGame\RhythmGame\Assets\Scripts\Ozi's Scene\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kimmi\Desktop\GameJamRhythmGame\GameJamRhythmGame\RhythmGame\Assets\Scripts\Ozi's Scene\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{890B8B70-000E-4AE2-B8AF-7EE81CD43C18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B480358-7CD3-4790-812F-0A7AC73FCE17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6210" yWindow="3195" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{A9B81C3C-755C-46FD-BFDE-D4E894C99174}"/>
+    <workbookView xWindow="-108" yWindow="252" windowWidth="23256" windowHeight="12816" activeTab="1" xr2:uid="{A9B81C3C-755C-46FD-BFDE-D4E894C99174}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -1443,21 +1443,21 @@
   <dimension ref="B1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="1.625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.59765625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.59765625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B2" s="39" t="s">
         <v>53</v>
       </c>
@@ -1467,7 +1467,7 @@
       <c r="F2" s="40"/>
       <c r="G2" s="41"/>
     </row>
-    <row r="3" spans="2:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="30" t="s">
         <v>115</v>
       </c>
@@ -1477,7 +1477,7 @@
       <c r="F3" s="31"/>
       <c r="G3" s="32"/>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B4" s="33"/>
       <c r="C4" s="34"/>
       <c r="D4" s="34"/>
@@ -1485,7 +1485,7 @@
       <c r="F4" s="34"/>
       <c r="G4" s="35"/>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B5" s="33"/>
       <c r="C5" s="34"/>
       <c r="D5" s="34"/>
@@ -1493,7 +1493,7 @@
       <c r="F5" s="34"/>
       <c r="G5" s="35"/>
     </row>
-    <row r="6" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B6" s="36"/>
       <c r="C6" s="37"/>
       <c r="D6" s="37"/>
@@ -1501,8 +1501,8 @@
       <c r="F6" s="37"/>
       <c r="G6" s="38"/>
     </row>
-    <row r="7" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="8" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B8" s="29" t="s">
         <v>104</v>
       </c>
@@ -1539,21 +1539,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B362864F-EB80-4CB1-87B1-BB77F0277502}">
   <dimension ref="B1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="1.625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="1.59765625" style="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.3984375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:4" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="2:4" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B2" s="16" t="s">
         <v>103</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B3" s="17" t="s">
         <v>105</v>
       </c>
@@ -1575,7 +1575,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B4" s="18" t="s">
         <v>107</v>
       </c>
@@ -1586,7 +1586,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B5" s="19" t="s">
         <v>109</v>
       </c>
@@ -1597,7 +1597,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B6" s="18" t="s">
         <v>111</v>
       </c>
@@ -1608,7 +1608,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:4" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B7" s="20" t="s">
         <v>113</v>
       </c>
@@ -1629,23 +1629,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DE133DF-DAB9-4128-86E8-233557D3597C}">
   <dimension ref="B1:F22"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="1.625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="49.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.59765625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="49.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.19921875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="48.5" style="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1"/>
-    <col min="6" max="6" width="25.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="25.8984375" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B2" s="16" t="s">
         <v>54</v>
       </c>
@@ -1659,7 +1659,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="B3" s="17" t="s">
         <v>55</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="18" t="s">
         <v>58</v>
       </c>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="F4" s="43"/>
     </row>
-    <row r="5" spans="2:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="B5" s="19" t="s">
         <v>62</v>
       </c>
@@ -1697,7 +1697,7 @@
       </c>
       <c r="F5" s="43"/>
     </row>
-    <row r="6" spans="2:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" ht="35.4" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B6" s="18" t="s">
         <v>64</v>
       </c>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="F6" s="44"/>
     </row>
-    <row r="7" spans="2:6" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B7" s="19" t="s">
         <v>69</v>
       </c>
@@ -1721,7 +1721,7 @@
       </c>
       <c r="F7"/>
     </row>
-    <row r="8" spans="2:6" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="18" t="s">
         <v>68</v>
       </c>
@@ -1733,7 +1733,7 @@
       </c>
       <c r="F8"/>
     </row>
-    <row r="9" spans="2:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="B9" s="19" t="s">
         <v>66</v>
       </c>
@@ -1744,7 +1744,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="B10" s="18" t="s">
         <v>70</v>
       </c>
@@ -1755,7 +1755,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B11" s="19" t="s">
         <v>72</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B12" s="18" t="s">
         <v>76</v>
       </c>
@@ -1777,7 +1777,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B13" s="19" t="s">
         <v>79</v>
       </c>
@@ -1788,7 +1788,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="B14" s="18" t="s">
         <v>81</v>
       </c>
@@ -1799,7 +1799,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B15" s="19" t="s">
         <v>84</v>
       </c>
@@ -1810,7 +1810,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B16" s="18" t="s">
         <v>86</v>
       </c>
@@ -1821,7 +1821,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B17" s="19" t="s">
         <v>88</v>
       </c>
@@ -1832,7 +1832,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B18" s="18" t="s">
         <v>90</v>
       </c>
@@ -1843,7 +1843,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B19" s="19" t="s">
         <v>92</v>
       </c>
@@ -1854,7 +1854,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B20" s="18" t="s">
         <v>96</v>
       </c>
@@ -1865,7 +1865,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B21" s="19" t="s">
         <v>98</v>
       </c>
@@ -1876,7 +1876,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="33.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:4" ht="35.4" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B22" s="21" t="s">
         <v>101</v>
       </c>
@@ -1900,21 +1900,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{652DE35F-883C-46B6-847E-F5BA274CB4C1}">
   <dimension ref="B1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="1.625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="1.59765625" style="1" customWidth="1"/>
     <col min="2" max="2" width="24.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.3984375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:4" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="2:4" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B2" s="16" t="s">
         <v>30</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B3" s="17" t="s">
         <v>31</v>
       </c>
@@ -1936,7 +1936,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B4" s="18" t="s">
         <v>33</v>
       </c>
@@ -1947,7 +1947,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B5" s="19" t="s">
         <v>36</v>
       </c>
@@ -1958,7 +1958,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B6" s="18" t="s">
         <v>39</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="33" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="B7" s="22" t="s">
         <v>41</v>
       </c>
@@ -1980,7 +1980,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="33" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="B8" s="18" t="s">
         <v>44</v>
       </c>
@@ -1991,7 +1991,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B9" s="19" t="s">
         <v>47</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B10" s="18" t="s">
         <v>50</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="33.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:4" ht="35.4" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B11" s="20" t="s">
         <v>51</v>
       </c>
@@ -2034,19 +2034,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A880481A-6616-416C-B484-E5EFE4D599EB}">
   <dimension ref="B1:D13"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="1.625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="27.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="62.625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="1.59765625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.59765625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="62.59765625" style="1" customWidth="1"/>
     <col min="5" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:4" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="2:4" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
@@ -2057,7 +2059,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B3" s="17" t="s">
         <v>1</v>
       </c>
@@ -2068,7 +2070,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B4" s="18" t="s">
         <v>6</v>
       </c>
@@ -2079,7 +2081,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B5" s="19" t="s">
         <v>9</v>
       </c>
@@ -2090,7 +2092,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="33" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="B6" s="18" t="s">
         <v>12</v>
       </c>
@@ -2101,7 +2103,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="33" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="B7" s="19" t="s">
         <v>14</v>
       </c>
@@ -2112,7 +2114,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="33" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="B8" s="18" t="s">
         <v>16</v>
       </c>
@@ -2123,7 +2125,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" ht="52.2" x14ac:dyDescent="0.4">
       <c r="B9" s="19" t="s">
         <v>18</v>
       </c>
@@ -2134,7 +2136,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B10" s="18" t="s">
         <v>21</v>
       </c>
@@ -2145,7 +2147,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:4" ht="52.2" x14ac:dyDescent="0.4">
       <c r="B11" s="19" t="s">
         <v>23</v>
       </c>
@@ -2156,7 +2158,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="66" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:4" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="B12" s="18" t="s">
         <v>25</v>
       </c>
@@ -2167,7 +2169,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="50.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:4" ht="100.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B13" s="20" t="s">
         <v>27</v>
       </c>

</xml_diff>